<commit_message>
Project Files are Updated
</commit_message>
<xml_diff>
--- a/PROJECT_INTERVIEW/WebService Data Dictionary.xlsx
+++ b/PROJECT_INTERVIEW/WebService Data Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium_Study\SELENIUM_NOTES\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\APP_SP_NOTES\DAILY_NOTES\PROJECT_INTERVIEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA8F7EB-0070-48AD-BA74-09BD4B56E0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B0C5A1-6245-41C0-B626-400C3A9DC787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{62E0AE0B-F734-4650-AB67-6025CE3015E4}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,7 +637,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -676,6 +675,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FE5CE6-FFD0-46FD-82A3-5F50E17B89F2}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,11 +1008,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.4">
@@ -1024,7 +1025,7 @@
       <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="31" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1446,7 +1447,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1601,37 +1602,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="57.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="E3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
@@ -1639,310 +1640,310 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>2</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>4</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>5</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <v>6</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>7</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>8</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>9</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>10</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>11</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>12</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="14">
+      <c r="A17" s="13">
         <v>13</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="14">
+      <c r="A18" s="13">
         <v>14</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="14">
+      <c r="A19" s="13">
         <v>15</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="14">
+      <c r="A20" s="13">
         <v>16</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="14">
+      <c r="A21" s="13">
         <v>17</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="14">
+      <c r="A22" s="13">
         <v>18</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="14">
+      <c r="A23" s="13">
         <v>19</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="14">
+      <c r="A24" s="13">
         <v>20</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="14">
-        <v>21</v>
-      </c>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="13">
+        <v>21</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="14">
+      <c r="A26" s="13">
         <v>22</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1955,8 +1956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD54B983-8870-4E97-8523-6870C084920A}">
   <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1968,103 +1969,103 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="18"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>1</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>2</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>3</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2074,75 +2075,75 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="25" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="144" x14ac:dyDescent="0.35">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>1</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="23" t="s">
+      <c r="D13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>2</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="23" t="s">
+      <c r="D14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.35">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>3</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="23" t="s">
+      <c r="D15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2173,103 +2174,103 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="18"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="28" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="108" x14ac:dyDescent="0.35">
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>1</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="54" x14ac:dyDescent="0.35">
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>2</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="126" x14ac:dyDescent="0.35">
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>3</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="15" t="s">
+      <c r="E9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2279,75 +2280,75 @@
       </c>
     </row>
     <row r="11" spans="2:6" ht="54" x14ac:dyDescent="0.35">
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="234" x14ac:dyDescent="0.35">
-      <c r="B13" s="14">
+    <row r="13" spans="2:6" ht="90" x14ac:dyDescent="0.35">
+      <c r="B13" s="13">
         <v>1</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="23" t="s">
+      <c r="E13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="108" x14ac:dyDescent="0.35">
-      <c r="B14" s="14">
+    <row r="14" spans="2:6" ht="36" x14ac:dyDescent="0.35">
+      <c r="B14" s="13">
         <v>2</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="23" t="s">
+      <c r="E14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="22" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="162" x14ac:dyDescent="0.35">
-      <c r="B15" s="14">
+    <row r="15" spans="2:6" ht="54" x14ac:dyDescent="0.35">
+      <c r="B15" s="13">
         <v>3</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="23" t="s">
+      <c r="E15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2373,105 +2374,105 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
-      <c r="B3" s="30" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="21"/>
-      <c r="B4" s="29" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="14"/>
+      <c r="D6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2481,75 +2482,75 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="25" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="162" x14ac:dyDescent="0.35">
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <v>1</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="23" t="s">
+      <c r="E14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="22" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="108" x14ac:dyDescent="0.35">
-      <c r="B15" s="14">
+      <c r="B15" s="13">
         <v>2</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="23" t="s">
+      <c r="E15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="162" x14ac:dyDescent="0.35">
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <v>3</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="23" t="s">
+      <c r="E16" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2569,142 +2570,142 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
-      <c r="B3" s="29" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="126" x14ac:dyDescent="0.35">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>1</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="14"/>
+      <c r="D6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="13"/>
     </row>
     <row r="16" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="25" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="234" x14ac:dyDescent="0.35">
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>1</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="23" t="s">
+      <c r="E18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="22" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="108" x14ac:dyDescent="0.35">
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <v>2</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="23" t="s">
+      <c r="E19" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="22" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="162" x14ac:dyDescent="0.35">
-      <c r="B20" s="14">
+      <c r="B20" s="13">
         <v>3</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="23" t="s">
+      <c r="E20" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="22" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>